<commit_message>
Fixed Mastersheet score update after carryover run
</commit_message>
<xml_diff>
--- a/EXAMS_INTERNAL/BM/BM-COURSES/M-course-code-creditUnit.xlsx
+++ b/EXAMS_INTERNAL/BM/BM-COURSES/M-course-code-creditUnit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="420" windowWidth="18820" windowHeight="6810" activeTab="4"/>
+    <workbookView xWindow="320" yWindow="420" windowWidth="18820" windowHeight="6810" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="M-FIRST-YEAR-FIRST-SEMESTER" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,42 @@
     <sheet name="M-THIRD-YEAR-SECOND-SEMESTER" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_Hlk100596162" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$A$3</definedName>
+    <definedName name="_Hlk100596350" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$A$6</definedName>
+    <definedName name="_Hlk100596400" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$A$7</definedName>
+    <definedName name="_Hlk100596419" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$B$7</definedName>
+    <definedName name="_Hlk100596441" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$A$8</definedName>
+    <definedName name="_Hlk100596501" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$A$9</definedName>
+    <definedName name="_Hlk100596528" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$B$9</definedName>
+    <definedName name="_Hlk100596550" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$A$4</definedName>
+    <definedName name="_Hlk100596595" localSheetId="0">'M-FIRST-YEAR-FIRST-SEMESTER'!$A$5</definedName>
+    <definedName name="_Hlk100596925" localSheetId="1">'M-FIRST-YEAR-SECOND-SEMESTER'!$B$2</definedName>
+    <definedName name="_Hlk100596973" localSheetId="1">'M-FIRST-YEAR-SECOND-SEMESTER'!$B$3</definedName>
+    <definedName name="_Hlk100597059" localSheetId="1">'M-FIRST-YEAR-SECOND-SEMESTER'!$B$4</definedName>
+    <definedName name="_Hlk100597124" localSheetId="1">'M-FIRST-YEAR-SECOND-SEMESTER'!$B$5</definedName>
+    <definedName name="_Hlk100597166" localSheetId="1">'M-FIRST-YEAR-SECOND-SEMESTER'!$B$6</definedName>
+    <definedName name="_Hlk100597268" localSheetId="1">'M-FIRST-YEAR-SECOND-SEMESTER'!$B$8</definedName>
+    <definedName name="_Hlk100598303" localSheetId="2">'M-SECOND-YEAR-FIRST-SEMESTER'!$B$4</definedName>
+    <definedName name="_Hlk100598424" localSheetId="2">'M-SECOND-YEAR-FIRST-SEMESTER'!$B$5</definedName>
+    <definedName name="_Hlk100598470" localSheetId="2">'M-SECOND-YEAR-FIRST-SEMESTER'!$B$9</definedName>
+    <definedName name="_Hlk100598766" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!$B$2</definedName>
+    <definedName name="_Hlk100598896" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!$B$3</definedName>
+    <definedName name="_Hlk100598995" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!$B$4</definedName>
+    <definedName name="_Hlk100599096" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!$B$6</definedName>
+    <definedName name="_Hlk100599155" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!$B$7</definedName>
+    <definedName name="_Hlk100599194" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!$B$8</definedName>
+    <definedName name="_Hlk100599248" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!$B$10</definedName>
+    <definedName name="_Hlk100599399" localSheetId="4">'M-THIRD-YEAR-FIRST-SEMESTER'!$B$2</definedName>
+    <definedName name="_Hlk100599443" localSheetId="4">'M-THIRD-YEAR-FIRST-SEMESTER'!$B$3</definedName>
+    <definedName name="_Hlk100599536" localSheetId="4">'M-THIRD-YEAR-FIRST-SEMESTER'!$B$5</definedName>
+    <definedName name="_Hlk100599585" localSheetId="4">'M-THIRD-YEAR-FIRST-SEMESTER'!$B$6</definedName>
+    <definedName name="_Hlk100599675" localSheetId="4">'M-THIRD-YEAR-FIRST-SEMESTER'!$B$7</definedName>
+    <definedName name="_Hlk100599715" localSheetId="4">'M-THIRD-YEAR-FIRST-SEMESTER'!$B$8</definedName>
+    <definedName name="_Hlk100599862" localSheetId="5">'M-THIRD-YEAR-SECOND-SEMESTER'!$B$2</definedName>
+    <definedName name="_Hlk100599911" localSheetId="5">'M-THIRD-YEAR-SECOND-SEMESTER'!$B$3</definedName>
+    <definedName name="_Hlk100600110" localSheetId="5">'M-THIRD-YEAR-SECOND-SEMESTER'!$B$5</definedName>
+    <definedName name="_Hlk100600153" localSheetId="5">'M-THIRD-YEAR-SECOND-SEMESTER'!$B$6</definedName>
+    <definedName name="_Hlk100600200" localSheetId="5">'M-THIRD-YEAR-SECOND-SEMESTER'!$B$7</definedName>
     <definedName name="_Hlk114062847" localSheetId="3">'M-SECOND-YEAR-SECOND-SEMESTER'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -22,47 +58,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
-  <si>
-    <t>Anatomy &amp; Physiology I</t>
-  </si>
-  <si>
-    <t>Foundation of Nursing I</t>
-  </si>
-  <si>
-    <t>Introduction to Nursing Informatics</t>
-  </si>
-  <si>
-    <t>Nutrition</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
   <si>
     <t>Use of English</t>
   </si>
   <si>
-    <t xml:space="preserve">Applied Physics </t>
-  </si>
-  <si>
     <t>Applied Chemistry</t>
   </si>
   <si>
-    <t xml:space="preserve">Microbiology </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social and Behavioral Science </t>
-  </si>
-  <si>
-    <t>GNS111</t>
-  </si>
-  <si>
-    <t>GNS112</t>
-  </si>
-  <si>
-    <t>GNS113</t>
-  </si>
-  <si>
-    <t>GNS114</t>
-  </si>
-  <si>
     <t>GST111</t>
   </si>
   <si>
@@ -75,9 +78,6 @@
     <t>GST114</t>
   </si>
   <si>
-    <t>GST115</t>
-  </si>
-  <si>
     <t>COURSE CODE</t>
   </si>
   <si>
@@ -90,241 +90,307 @@
     <t>Anatomy and Physiology II</t>
   </si>
   <si>
-    <t>Foundation of Nursing II</t>
-  </si>
-  <si>
     <t>Medical-Surgical Nursing I</t>
   </si>
   <si>
     <t>Primary Health Care I</t>
   </si>
   <si>
-    <t>Pharmacology I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nursing Ethics and Jurisprudence </t>
-  </si>
-  <si>
-    <t>Dietetics</t>
-  </si>
-  <si>
-    <t>Hospital-Based Nursing Practicum I</t>
-  </si>
-  <si>
-    <t>GNS121</t>
-  </si>
-  <si>
-    <t>GNS122</t>
-  </si>
-  <si>
-    <t>GNS123</t>
-  </si>
-  <si>
-    <t>GNS124</t>
-  </si>
-  <si>
-    <t>GNS125</t>
-  </si>
-  <si>
-    <t>GNS126</t>
-  </si>
-  <si>
-    <t>GNS127</t>
-  </si>
-  <si>
-    <t>GNS128</t>
-  </si>
-  <si>
-    <t>GNS 211</t>
-  </si>
-  <si>
-    <t>Anatomy and Physiology III</t>
-  </si>
-  <si>
-    <t>GNS 212</t>
-  </si>
-  <si>
-    <t>Foundation of Nursing III</t>
-  </si>
-  <si>
-    <t>GNS 213</t>
-  </si>
-  <si>
     <t>Medical-Surgical Nursing II</t>
   </si>
   <si>
-    <t>GNS 214</t>
-  </si>
-  <si>
-    <t>Primary Health Care II</t>
-  </si>
-  <si>
-    <t>GNS 215</t>
-  </si>
-  <si>
-    <t>Pharmacology II</t>
-  </si>
-  <si>
-    <t>GNS 216</t>
-  </si>
-  <si>
     <t>Reproductive Health I</t>
   </si>
   <si>
-    <t>GNS 217</t>
-  </si>
-  <si>
-    <t>Research &amp; Statistics I</t>
-  </si>
-  <si>
-    <t>GNS 218</t>
-  </si>
-  <si>
-    <t>Hospital-Based Nursing Practicum II</t>
-  </si>
-  <si>
-    <t>Foundation of Nursing IV</t>
-  </si>
-  <si>
-    <t>Medical-Surgical Nursing III</t>
-  </si>
-  <si>
-    <t>Pharmacology III</t>
-  </si>
-  <si>
     <t>Research and Statistics II</t>
   </si>
   <si>
-    <t>Community Health Nursing I</t>
-  </si>
-  <si>
-    <t>Reproductive Health II</t>
-  </si>
-  <si>
-    <t>Introduction to Professional Writing and Seminar in Nursing</t>
-  </si>
-  <si>
-    <t>Hospital-Based Nursing Practicum III</t>
-  </si>
-  <si>
-    <t>Politics and Governance in Nursing</t>
-  </si>
-  <si>
-    <t>GNS221</t>
-  </si>
-  <si>
-    <t>GNS222</t>
-  </si>
-  <si>
-    <t>GNS223</t>
-  </si>
-  <si>
-    <t>GNS224</t>
-  </si>
-  <si>
-    <t>GNS225</t>
-  </si>
-  <si>
-    <t>GNS226</t>
-  </si>
-  <si>
-    <t>GNS227</t>
-  </si>
-  <si>
-    <t>GNS228</t>
-  </si>
-  <si>
-    <t>GST221</t>
-  </si>
-  <si>
-    <t>Medical-Surgical Nursing IV</t>
-  </si>
-  <si>
-    <t>Reproductive Health III</t>
-  </si>
-  <si>
-    <t>Community Health Nursing II</t>
-  </si>
-  <si>
     <t>Mental Health-Psychiatric Nursing</t>
   </si>
   <si>
-    <t>Emergency and Disaster Nursing</t>
-  </si>
-  <si>
-    <t>Quality Improvement in Healthcare and Patient Safety</t>
-  </si>
-  <si>
-    <t>Use of English 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community-Based Practice </t>
-  </si>
-  <si>
-    <t>GNS311</t>
-  </si>
-  <si>
-    <t>GNS312</t>
-  </si>
-  <si>
-    <t>GNS313</t>
-  </si>
-  <si>
-    <t>GNS314</t>
-  </si>
-  <si>
-    <t>GNS315</t>
-  </si>
-  <si>
-    <t>GNS316</t>
-  </si>
-  <si>
-    <t>GST311</t>
-  </si>
-  <si>
-    <t>GNS317</t>
-  </si>
-  <si>
-    <t>Medical-Surgical Nursing V</t>
-  </si>
-  <si>
     <t>Research Project</t>
   </si>
   <si>
-    <t>Home Health Care Nursing</t>
-  </si>
-  <si>
     <t>Principles of Management and Teaching</t>
   </si>
   <si>
-    <t>Health Economics</t>
-  </si>
-  <si>
-    <t>Entrepreneurship in Nursing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital-Based Nursing Practicum    IV </t>
-  </si>
-  <si>
-    <t>GNS321</t>
-  </si>
-  <si>
-    <t>GNS322</t>
-  </si>
-  <si>
-    <t>GNS323</t>
-  </si>
-  <si>
     <t>GST321</t>
   </si>
   <si>
-    <t>GST322</t>
-  </si>
-  <si>
-    <t>GST323</t>
-  </si>
-  <si>
-    <t>GNS324</t>
+    <t>Foundations of Nursing I</t>
+  </si>
+  <si>
+    <t>Anatomy and Physiology I</t>
+  </si>
+  <si>
+    <t>Nutrition and Dietetics</t>
+  </si>
+  <si>
+    <t>Applied Physics</t>
+  </si>
+  <si>
+    <t>Social and Behavioural Science</t>
+  </si>
+  <si>
+    <t>Practicum Examination</t>
+  </si>
+  <si>
+    <t>MID111</t>
+  </si>
+  <si>
+    <t>MID112</t>
+  </si>
+  <si>
+    <t>MID113</t>
+  </si>
+  <si>
+    <t>MID114</t>
+  </si>
+  <si>
+    <t>MID115</t>
+  </si>
+  <si>
+    <t>MID121</t>
+  </si>
+  <si>
+    <t>MID122</t>
+  </si>
+  <si>
+    <t>MID123</t>
+  </si>
+  <si>
+    <t>MID124</t>
+  </si>
+  <si>
+    <t>MID125</t>
+  </si>
+  <si>
+    <t>MID126</t>
+  </si>
+  <si>
+    <t>MID127</t>
+  </si>
+  <si>
+    <t>GST121</t>
+  </si>
+  <si>
+    <t>GST122</t>
+  </si>
+  <si>
+    <t>MID128</t>
+  </si>
+  <si>
+    <t>Foundations of Nursing II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Health Care II </t>
+  </si>
+  <si>
+    <t>Pharmacology in Midwifery I</t>
+  </si>
+  <si>
+    <t>Nutrition and Dietetics II</t>
+  </si>
+  <si>
+    <t>Hospital-Based Midwifery Practicum I</t>
+  </si>
+  <si>
+    <t>Microbiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Nursing Informatics </t>
+  </si>
+  <si>
+    <t>Objective Structural Clinical Examination I</t>
+  </si>
+  <si>
+    <t>MID211</t>
+  </si>
+  <si>
+    <t>MID212</t>
+  </si>
+  <si>
+    <t>MID213</t>
+  </si>
+  <si>
+    <t>MID214</t>
+  </si>
+  <si>
+    <t>MID215</t>
+  </si>
+  <si>
+    <t>MID216</t>
+  </si>
+  <si>
+    <t>GST211</t>
+  </si>
+  <si>
+    <t>GST212</t>
+  </si>
+  <si>
+    <t>MID217</t>
+  </si>
+  <si>
+    <t>Child Health</t>
+  </si>
+  <si>
+    <t>Home-Health Care Nursing</t>
+  </si>
+  <si>
+    <t>Primary Health Care III</t>
+  </si>
+  <si>
+    <t>Entrepreneurship in Midwifery</t>
+  </si>
+  <si>
+    <t>Objective Structural Clinical Examination II</t>
+  </si>
+  <si>
+    <t>Community-Based Midwifery Practicum I</t>
+  </si>
+  <si>
+    <t>MID221</t>
+  </si>
+  <si>
+    <t>MID222</t>
+  </si>
+  <si>
+    <t>MID223</t>
+  </si>
+  <si>
+    <t>MID224</t>
+  </si>
+  <si>
+    <t>MID225</t>
+  </si>
+  <si>
+    <t>MID226</t>
+  </si>
+  <si>
+    <t>MID227</t>
+  </si>
+  <si>
+    <t>MID228</t>
+  </si>
+  <si>
+    <t>MID229</t>
+  </si>
+  <si>
+    <t>MID230</t>
+  </si>
+  <si>
+    <t>Fundamentals of Midwifery Practice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applied Anatomy and Physiology </t>
+  </si>
+  <si>
+    <t>Normal Midwifery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complicated Midwifery I </t>
+  </si>
+  <si>
+    <t>Pharmacology in Midwifery II</t>
+  </si>
+  <si>
+    <t>Infant I</t>
+  </si>
+  <si>
+    <t>Community Midwifery</t>
+  </si>
+  <si>
+    <t>Research and Statistics I</t>
+  </si>
+  <si>
+    <t>Hospital-based Midwifery Practicum II</t>
+  </si>
+  <si>
+    <t>Objective Structural Clinical Examination III</t>
+  </si>
+  <si>
+    <t>MID311</t>
+  </si>
+  <si>
+    <t>MID312</t>
+  </si>
+  <si>
+    <t>MID313</t>
+  </si>
+  <si>
+    <t>MID314</t>
+  </si>
+  <si>
+    <t>MID315</t>
+  </si>
+  <si>
+    <t>MID316</t>
+  </si>
+  <si>
+    <t>MID317</t>
+  </si>
+  <si>
+    <t>MID318</t>
+  </si>
+  <si>
+    <t>Infant II</t>
+  </si>
+  <si>
+    <t>Family Planning</t>
+  </si>
+  <si>
+    <t>Complicated Midwifery II</t>
+  </si>
+  <si>
+    <t>Seminar in Midwifery I</t>
+  </si>
+  <si>
+    <t>Community-based Midwifery Practicum II</t>
+  </si>
+  <si>
+    <t>Objective Structural Clinical Examination IV</t>
+  </si>
+  <si>
+    <t>MID321</t>
+  </si>
+  <si>
+    <t>MID322</t>
+  </si>
+  <si>
+    <t>MID323</t>
+  </si>
+  <si>
+    <t>MID324</t>
+  </si>
+  <si>
+    <t>MID325</t>
+  </si>
+  <si>
+    <t>MID326</t>
+  </si>
+  <si>
+    <t>MID327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reproductive Health II </t>
+  </si>
+  <si>
+    <t>Quality Improvement in Healthcare and Patient safety</t>
+  </si>
+  <si>
+    <t>Care in Humanitarian setting</t>
+  </si>
+  <si>
+    <t>Expectant Family Care Project</t>
+  </si>
+  <si>
+    <t>Seminar in Midwifery II</t>
+  </si>
+  <si>
+    <t>School Health Programme</t>
+  </si>
+  <si>
+    <t>Objective Structural Clinical Examination V</t>
   </si>
 </sst>
 </file>
@@ -669,7 +735,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,21 +747,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>4</v>
@@ -703,21 +769,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -725,10 +791,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -736,10 +802,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -747,10 +813,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -758,21 +824,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -780,13 +846,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -797,69 +863,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -867,21 +933,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -889,10 +955,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -900,12 +966,34 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1">
         <v>4</v>
       </c>
     </row>
@@ -916,36 +1004,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.36328125" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -953,10 +1041,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -964,21 +1052,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -986,10 +1074,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -997,34 +1085,45 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1035,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,43 +1149,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1094,21 +1193,21 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1116,21 +1215,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1138,24 +1237,35 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1167,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1180,21 +1290,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -1202,10 +1312,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -1213,21 +1323,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1235,43 +1345,43 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -1284,36 +1394,36 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7265625" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -1321,21 +1431,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1343,21 +1453,21 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1365,10 +1475,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -1376,12 +1486,23 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>